<commit_message>
tablas y evaluaciones todas
</commit_message>
<xml_diff>
--- a/files/respuestas/2023/respuestas_2023.xlsx
+++ b/files/respuestas/2023/respuestas_2023.xlsx
@@ -44604,16 +44604,16 @@
         <v>0</v>
       </c>
       <c r="CN72">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="CO72">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="CP72">
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="CQ72">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="CR72">
         <v>0</v>

</xml_diff>

<commit_message>
Alpha 1.3 con errores conocidos eliminados. Falta corregir tabla de resultados mas adelante
</commit_message>
<xml_diff>
--- a/files/respuestas/2023/respuestas_2023.xlsx
+++ b/files/respuestas/2023/respuestas_2023.xlsx
@@ -18016,7 +18016,7 @@
         <v>0.88</v>
       </c>
       <c r="EN27" t="n">
-        <v>1.89</v>
+        <v>1.85</v>
       </c>
       <c r="EO27" t="n">
         <v>0.55</v>
@@ -18028,7 +18028,7 @@
         <v>0.1364</v>
       </c>
       <c r="ER27" t="n">
-        <v>3.03</v>
+        <v>2.99</v>
       </c>
       <c r="ES27" t="n">
         <v>0</v>
@@ -18046,22 +18046,22 @@
         <v>1.5</v>
       </c>
       <c r="EX27" t="n">
-        <v>0</v>
+        <v>0.76</v>
       </c>
       <c r="EY27" t="n">
         <v>1.4</v>
       </c>
       <c r="EZ27" t="n">
-        <v>1.4</v>
+        <v>2.16</v>
       </c>
       <c r="FA27" t="n">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="FB27" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="FC27" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="FD27" t="n">
         <v>0</v>
@@ -18070,22 +18070,22 @@
         <v>0</v>
       </c>
       <c r="FF27" t="n">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="FG27" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="FH27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="FI27" t="n">
-        <v>0</v>
+        <v>0.91</v>
       </c>
       <c r="FJ27" t="n">
-        <v>0</v>
+        <v>2.04</v>
       </c>
       <c r="FK27" t="n">
-        <v>0</v>
+        <v>11.45</v>
       </c>
       <c r="FL27" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Reorganización de todas las funciones dentro de stats
</commit_message>
<xml_diff>
--- a/files/respuestas/2023/respuestas_2023.xlsx
+++ b/files/respuestas/2023/respuestas_2023.xlsx
@@ -22460,52 +22460,52 @@
         <v>0</v>
       </c>
       <c r="CN34" t="n">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="CO34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CP34" t="n">
-        <v>0</v>
+        <v>1.32</v>
       </c>
       <c r="CQ34" t="n">
-        <v>0</v>
+        <v>3.52</v>
       </c>
       <c r="CR34" t="n">
         <v>0</v>
       </c>
       <c r="CS34" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="CT34" t="n">
-        <v>0</v>
+        <v>1.1</v>
       </c>
       <c r="CU34" t="n">
-        <v>0</v>
+        <v>2.6</v>
       </c>
       <c r="CV34" t="n">
         <v>0</v>
       </c>
       <c r="CW34" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="CX34" t="n">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="CY34" t="n">
-        <v>0</v>
+        <v>1.9</v>
       </c>
       <c r="CZ34" t="n">
         <v>0</v>
       </c>
       <c r="DA34" t="n">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="DB34" t="n">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="DC34" t="n">
-        <v>0</v>
+        <v>1.95</v>
       </c>
       <c r="DD34" t="n">
         <v>0</v>
@@ -22514,70 +22514,70 @@
         <v>0</v>
       </c>
       <c r="DF34" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="DG34" t="n">
-        <v>0</v>
+        <v>1.9</v>
       </c>
       <c r="DH34" t="n">
-        <v>0</v>
+        <v>3.9</v>
       </c>
       <c r="DI34" t="n">
         <v>0</v>
       </c>
       <c r="DJ34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DK34" t="n">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="DL34" t="n">
-        <v>0</v>
+        <v>2.8</v>
       </c>
       <c r="DM34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DN34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DO34" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="DP34" t="n">
-        <v>0</v>
+        <v>0.43</v>
       </c>
       <c r="DQ34" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="DR34" t="n">
-        <v>0</v>
+        <v>0.83</v>
       </c>
       <c r="DS34" t="n">
-        <v>0</v>
+        <v>1.4</v>
       </c>
       <c r="DT34" t="n">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="DU34" t="n">
-        <v>0</v>
+        <v>2.15</v>
       </c>
       <c r="DV34" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="DW34" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="DX34" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="DY34" t="n">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="DZ34" t="n">
         <v>0</v>
       </c>
       <c r="EA34" t="n">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="EB34" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Fixes a tabla de seguimiento a puntajes
</commit_message>
<xml_diff>
--- a/files/respuestas/2023/respuestas_2023.xlsx
+++ b/files/respuestas/2023/respuestas_2023.xlsx
@@ -22571,55 +22571,55 @@
         <v>0.7</v>
       </c>
       <c r="DY34" t="n">
-        <v>0.15</v>
+        <v>0.4</v>
       </c>
       <c r="DZ34" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="EA34" t="n">
-        <v>0.15</v>
+        <v>1</v>
       </c>
       <c r="EB34" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="EC34" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="ED34" t="n">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="EE34" t="n">
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="EF34" t="n">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="EG34" t="n">
-        <v>0</v>
+        <v>2.45</v>
       </c>
       <c r="EH34" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EI34" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="EJ34" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="EK34" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EL34" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="EM34" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EN34" t="n">
         <v>0</v>
       </c>
       <c r="EO34" t="n">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="EP34" t="n">
         <v>0</v>
@@ -22628,7 +22628,7 @@
         <v>0</v>
       </c>
       <c r="ER34" t="n">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="ES34" t="n">
         <v>0</v>

</xml_diff>